<commit_message>
register user section finished
</commit_message>
<xml_diff>
--- a/LocalizableVariables.xlsx
+++ b/LocalizableVariables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/care/Documents/Projeler/TwitterClone/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12591B9B-ACE5-D645-8A65-597FB721E849}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0E77DAA-6B71-D343-B9D3-41CEB72CDFAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30880" yWindow="3320" windowWidth="28300" windowHeight="16120" xr2:uid="{72E0D217-C508-DF4E-A1A6-4536DDF70BEF}"/>
+    <workbookView xWindow="38180" yWindow="4100" windowWidth="28300" windowHeight="16120" xr2:uid="{72E0D217-C508-DF4E-A1A6-4536DDF70BEF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sayfa1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="73">
   <si>
     <t>Value</t>
   </si>
@@ -144,6 +144,117 @@
   </si>
   <si>
     <t>Atla</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>Eposta</t>
+  </si>
+  <si>
+    <t>Parola</t>
+  </si>
+  <si>
+    <t>forgot_password</t>
+  </si>
+  <si>
+    <t>Parolanı unuttun mu?</t>
+  </si>
+  <si>
+    <t>Forgot Password?</t>
+  </si>
+  <si>
+    <t>sign_in</t>
+  </si>
+  <si>
+    <t>Sign In</t>
+  </si>
+  <si>
+    <t>Giriş</t>
+  </si>
+  <si>
+    <t>Don't have an account?</t>
+  </si>
+  <si>
+    <t>Hesabın yok mu?</t>
+  </si>
+  <si>
+    <t>Sign Up</t>
+  </si>
+  <si>
+    <t>Kayıt ol</t>
+  </si>
+  <si>
+    <t>dont_have_an_account</t>
+  </si>
+  <si>
+    <t>sign_up</t>
+  </si>
+  <si>
+    <t>Welcome back</t>
+  </si>
+  <si>
+    <t>hello</t>
+  </si>
+  <si>
+    <t>welcome_back</t>
+  </si>
+  <si>
+    <t>create_your_account</t>
+  </si>
+  <si>
+    <t>get_started</t>
+  </si>
+  <si>
+    <t>Hello,</t>
+  </si>
+  <si>
+    <t>Merhaba,</t>
+  </si>
+  <si>
+    <t>Tekrar hoşgeldin</t>
+  </si>
+  <si>
+    <t>Create your account</t>
+  </si>
+  <si>
+    <t>Hesap Oluştur</t>
+  </si>
+  <si>
+    <t>Get started.</t>
+  </si>
+  <si>
+    <t>Başlayalım.</t>
+  </si>
+  <si>
+    <t>username</t>
+  </si>
+  <si>
+    <t>fullname</t>
+  </si>
+  <si>
+    <t>Username</t>
+  </si>
+  <si>
+    <t>Fullname</t>
+  </si>
+  <si>
+    <t>Kullanıcı adı</t>
+  </si>
+  <si>
+    <t>Tam ad</t>
+  </si>
+  <si>
+    <t>Already have an account</t>
+  </si>
+  <si>
+    <t>Zaten hesabınız var mı?</t>
+  </si>
+  <si>
+    <t>already_have_an_account</t>
   </si>
 </sst>
 </file>
@@ -526,10 +637,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A35C287-0029-D543-8BC3-8066F36528B2}">
-  <dimension ref="A1:F21"/>
+  <dimension ref="A1:F28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="F28" sqref="F2:F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -587,11 +698,11 @@
         <v>10</v>
       </c>
       <c r="E3" s="1" t="str">
-        <f t="shared" ref="E3:E21" si="0">""""&amp;$A3&amp;""""&amp;" = "&amp;""""&amp;B3&amp;""""&amp;";"</f>
+        <f t="shared" ref="E3:E28" si="0">""""&amp;$A3&amp;""""&amp;" = "&amp;""""&amp;B3&amp;""""&amp;";"</f>
         <v>"following" = "Following";</v>
       </c>
       <c r="F3" s="1" t="str">
-        <f t="shared" ref="F3:F21" si="1">""""&amp;$A3&amp;""""&amp;" = "&amp;""""&amp;C3&amp;""""&amp;";"</f>
+        <f t="shared" ref="F3:F28" si="1">""""&amp;$A3&amp;""""&amp;" = "&amp;""""&amp;C3&amp;""""&amp;";"</f>
         <v>"following" = "Takip Edilen";</v>
       </c>
     </row>
@@ -835,63 +946,252 @@
       </c>
     </row>
     <row r="16" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="str">
+        <f t="shared" ref="A16:A17" si="3">LOWER(B16)</f>
+        <v>email</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>38</v>
+      </c>
       <c r="E16" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>"" = "";</v>
+        <v>"email" = "Email";</v>
       </c>
       <c r="F16" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>"" = "";</v>
-      </c>
-    </row>
-    <row r="17" spans="5:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+        <v>"email" = "Eposta";</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>password</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>39</v>
+      </c>
       <c r="E17" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>"" = "";</v>
+        <v>"password" = "Password";</v>
       </c>
       <c r="F17" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>"" = "";</v>
-      </c>
-    </row>
-    <row r="18" spans="5:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+        <v>"password" = "Parola";</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>41</v>
+      </c>
       <c r="E18" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>"" = "";</v>
+        <v>"forgot_password" = "Forgot Password?";</v>
       </c>
       <c r="F18" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>"" = "";</v>
-      </c>
-    </row>
-    <row r="19" spans="5:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+        <v>"forgot_password" = "Parolanı unuttun mu?";</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>45</v>
+      </c>
       <c r="E19" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>"" = "";</v>
+        <v>"sign_in" = "Sign In";</v>
       </c>
       <c r="F19" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>"" = "";</v>
-      </c>
-    </row>
-    <row r="20" spans="5:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+        <v>"sign_in" = "Giriş";</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>47</v>
+      </c>
       <c r="E20" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>"" = "";</v>
+        <v>"dont_have_an_account" = "Don't have an account?";</v>
       </c>
       <c r="F20" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>"" = "";</v>
-      </c>
-    </row>
-    <row r="21" spans="5:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+        <v>"dont_have_an_account" = "Hesabın yok mu?";</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>49</v>
+      </c>
       <c r="E21" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>"" = "";</v>
+        <v>"sign_up" = "Sign Up";</v>
       </c>
       <c r="F21" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>"" = "";</v>
+        <v>"sign_up" = "Kayıt ol";</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E22" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>"hello" = "Hello,";</v>
+      </c>
+      <c r="F22" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>"hello" = "Merhaba,";</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E23" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>"welcome_back" = "Welcome back";</v>
+      </c>
+      <c r="F23" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>"welcome_back" = "Tekrar hoşgeldin";</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E24" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>"create_your_account" = "Create your account";</v>
+      </c>
+      <c r="F24" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>"create_your_account" = "Hesap Oluştur";</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E25" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>"get_started" = "Get started.";</v>
+      </c>
+      <c r="F25" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>"get_started" = "Başlayalım.";</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="E26" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>"username" = "Username";</v>
+      </c>
+      <c r="F26" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>"username" = "Kullanıcı adı";</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="E27" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>"fullname" = "Fullname";</v>
+      </c>
+      <c r="F27" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>"fullname" = "Tam ad";</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="E28" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>"already_have_an_account" = "Already have an account";</v>
+      </c>
+      <c r="F28" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>"already_have_an_account" = "Zaten hesabınız var mı?";</v>
       </c>
     </row>
   </sheetData>

</xml_diff>